<commit_message>
finished bom, exported gerbers
</commit_message>
<xml_diff>
--- a/pcb/haptic-control-bom.xlsx
+++ b/pcb/haptic-control-bom.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26846" windowHeight="11634"/>
+    <workbookView windowWidth="19095" windowHeight="12375"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="285">
   <si>
     <t>Device</t>
   </si>
@@ -838,28 +838,31 @@
     <t>U1</t>
   </si>
   <si>
-    <t>OUT OF STOCK</t>
-  </si>
-  <si>
     <t>Microchip Technology / Micrel</t>
   </si>
   <si>
-    <t>MIC23159YML-T5</t>
-  </si>
-  <si>
-    <t>https://eu.mouser.com/ProductDetail/Microchip-Technology-Micrel/MIC23159YML-T5?qs=sGAEpiMZZMvJkDqKJH80dGTtZZsskylho90qXbUH5kI%3D</t>
+    <t>MIC23158YML-T5</t>
+  </si>
+  <si>
+    <t>https://eu.mouser.com/ProductDetail/Microchip-Technology-Micrel/MIC23158YML-T5?qs=sGAEpiMZZMvJkDqKJH80dI1ScUCxw4n%2Fo5KJgdGCgUI%3D</t>
   </si>
   <si>
     <t>flash</t>
   </si>
   <si>
-    <t>4Mb</t>
+    <t>8Mbit</t>
   </si>
   <si>
     <t>WSOIC8</t>
   </si>
   <si>
-    <t>to be determined</t>
+    <t>Winbond</t>
+  </si>
+  <si>
+    <t>W25Q80DVSSIG</t>
+  </si>
+  <si>
+    <t>https://eu.mouser.com/ProductDetail/Winbond/W25Q80DVSSIG?qs=sGAEpiMZZMve4%2FbfQkoj%252BIdm5BjjR50fMw1zyWOlPKQ%3D</t>
   </si>
   <si>
     <t>Total:</t>
@@ -874,9 +877,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -929,24 +932,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -960,11 +955,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -976,9 +978,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -993,23 +1002,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1017,13 +1010,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1044,16 +1030,33 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1086,7 +1089,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1098,19 +1107,115 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1128,25 +1233,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1158,97 +1245,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1457,15 +1460,6 @@
       </diagonal>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1484,48 +1478,25 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -1546,11 +1517,43 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1559,55 +1562,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="21" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1616,64 +1619,64 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="12" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="19" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="18" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1682,29 +1685,29 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1768,22 +1771,10 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="18" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="19" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="18" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="19" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="19" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="18" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="18" applyBorder="1" applyAlignment="1">
@@ -1795,20 +1786,14 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="19" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="18" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="18" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="3" xfId="48" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="18" applyFont="1" applyBorder="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="18" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="19" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="3" xfId="18" applyFont="1" applyBorder="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="19" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
@@ -1897,10 +1882,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="D3DAE3"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FCFCFC"/>
+        <a:sysClr val="window" lastClr="404552"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -2152,37 +2137,37 @@
   <sheetPr/>
   <dimension ref="A1:OR70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J29" workbookViewId="0">
-      <selection activeCell="N62" sqref="N62"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7972027972028" defaultRowHeight="14.95"/>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
   <cols>
-    <col min="1" max="1" width="16.0629370629371" style="3" customWidth="1"/>
-    <col min="2" max="2" width="15.5734265734266" style="4" customWidth="1"/>
-    <col min="3" max="3" width="10.8601398601399" style="5" customWidth="1"/>
-    <col min="4" max="4" width="23.8321678321678" style="4" customWidth="1"/>
-    <col min="5" max="5" width="22.3426573426573" style="5" customWidth="1"/>
-    <col min="6" max="6" width="27.2447552447552" style="4" customWidth="1"/>
-    <col min="7" max="7" width="21.5384615384615" style="5" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="7.38461538461539" style="4" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="16.7622377622378" style="5" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="13.1608391608392" style="4" customWidth="1"/>
-    <col min="11" max="11" width="22.8671328671329" style="5" customWidth="1"/>
-    <col min="12" max="12" width="9.96503496503496" style="4" customWidth="1"/>
-    <col min="13" max="13" width="14.5594405594406" style="5" customWidth="1"/>
-    <col min="14" max="14" width="5.37762237762238" style="4" customWidth="1"/>
-    <col min="15" max="15" width="10.3706293706294" style="5" customWidth="1"/>
-    <col min="16" max="16" width="11.8671328671329" style="4" customWidth="1"/>
-    <col min="17" max="17" width="13.4685314685315" style="5" customWidth="1"/>
-    <col min="18" max="18" width="29.6083916083916" style="4" customWidth="1"/>
-    <col min="19" max="19" width="32.7062937062937" style="5" customWidth="1"/>
-    <col min="20" max="20" width="12.972027972028" style="4" customWidth="1"/>
-    <col min="21" max="21" width="8.7972027972028" style="6"/>
-    <col min="22" max="408" width="8.7972027972028" style="7"/>
+    <col min="1" max="1" width="16.0666666666667" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.575" style="4" customWidth="1"/>
+    <col min="3" max="3" width="10.8583333333333" style="5" customWidth="1"/>
+    <col min="4" max="4" width="95.375" style="4" customWidth="1"/>
+    <col min="5" max="5" width="22.3416666666667" style="5" customWidth="1"/>
+    <col min="6" max="6" width="27.2416666666667" style="4" customWidth="1"/>
+    <col min="7" max="7" width="22.75" style="5" customWidth="1"/>
+    <col min="8" max="8" width="8.25" style="4" customWidth="1"/>
+    <col min="9" max="9" width="19.125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="13.1583333333333" style="4" customWidth="1"/>
+    <col min="11" max="11" width="22.8666666666667" style="5" customWidth="1"/>
+    <col min="12" max="12" width="9.96666666666667" style="4" customWidth="1"/>
+    <col min="13" max="13" width="14.5583333333333" style="5" customWidth="1"/>
+    <col min="14" max="14" width="5.375" style="4" customWidth="1"/>
+    <col min="15" max="15" width="10.3666666666667" style="5" customWidth="1"/>
+    <col min="16" max="16" width="11.8666666666667" style="4" customWidth="1"/>
+    <col min="17" max="17" width="13.4666666666667" style="5" customWidth="1"/>
+    <col min="18" max="18" width="29.6083333333333" style="4" customWidth="1"/>
+    <col min="19" max="19" width="32.7083333333333" style="5" customWidth="1"/>
+    <col min="20" max="20" width="12.975" style="4" customWidth="1"/>
+    <col min="21" max="21" width="8.8" style="6"/>
+    <col min="22" max="408" width="8.8" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="20.7" spans="1:408">
+    <row r="1" s="1" customFormat="1" ht="18" spans="1:408">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -2243,396 +2228,396 @@
       <c r="T1" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="36"/>
-      <c r="V1" s="37"/>
-      <c r="W1" s="37"/>
-      <c r="X1" s="37"/>
-      <c r="Y1" s="37"/>
-      <c r="Z1" s="37"/>
-      <c r="AA1" s="37"/>
-      <c r="AB1" s="37"/>
-      <c r="AC1" s="37"/>
-      <c r="AD1" s="37"/>
-      <c r="AE1" s="37"/>
-      <c r="AF1" s="37"/>
-      <c r="AG1" s="37"/>
-      <c r="AH1" s="37"/>
-      <c r="AI1" s="37"/>
-      <c r="AJ1" s="37"/>
-      <c r="AK1" s="37"/>
-      <c r="AL1" s="37"/>
-      <c r="AM1" s="37"/>
-      <c r="AN1" s="37"/>
-      <c r="AO1" s="37"/>
-      <c r="AP1" s="37"/>
-      <c r="AQ1" s="37"/>
-      <c r="AR1" s="37"/>
-      <c r="AS1" s="37"/>
-      <c r="AT1" s="37"/>
-      <c r="AU1" s="37"/>
-      <c r="AV1" s="37"/>
-      <c r="AW1" s="37"/>
-      <c r="AX1" s="37"/>
-      <c r="AY1" s="37"/>
-      <c r="AZ1" s="37"/>
-      <c r="BA1" s="37"/>
-      <c r="BB1" s="37"/>
-      <c r="BC1" s="37"/>
-      <c r="BD1" s="37"/>
-      <c r="BE1" s="37"/>
-      <c r="BF1" s="37"/>
-      <c r="BG1" s="37"/>
-      <c r="BH1" s="37"/>
-      <c r="BI1" s="37"/>
-      <c r="BJ1" s="37"/>
-      <c r="BK1" s="37"/>
-      <c r="BL1" s="37"/>
-      <c r="BM1" s="37"/>
-      <c r="BN1" s="37"/>
-      <c r="BO1" s="37"/>
-      <c r="BP1" s="37"/>
-      <c r="BQ1" s="37"/>
-      <c r="BR1" s="37"/>
-      <c r="BS1" s="37"/>
-      <c r="BT1" s="37"/>
-      <c r="BU1" s="37"/>
-      <c r="BV1" s="37"/>
-      <c r="BW1" s="37"/>
-      <c r="BX1" s="37"/>
-      <c r="BY1" s="37"/>
-      <c r="BZ1" s="37"/>
-      <c r="CA1" s="37"/>
-      <c r="CB1" s="37"/>
-      <c r="CC1" s="37"/>
-      <c r="CD1" s="37"/>
-      <c r="CE1" s="37"/>
-      <c r="CF1" s="37"/>
-      <c r="CG1" s="37"/>
-      <c r="CH1" s="37"/>
-      <c r="CI1" s="37"/>
-      <c r="CJ1" s="37"/>
-      <c r="CK1" s="37"/>
-      <c r="CL1" s="37"/>
-      <c r="CM1" s="37"/>
-      <c r="CN1" s="37"/>
-      <c r="CO1" s="37"/>
-      <c r="CP1" s="37"/>
-      <c r="CQ1" s="37"/>
-      <c r="CR1" s="37"/>
-      <c r="CS1" s="37"/>
-      <c r="CT1" s="37"/>
-      <c r="CU1" s="37"/>
-      <c r="CV1" s="37"/>
-      <c r="CW1" s="37"/>
-      <c r="CX1" s="37"/>
-      <c r="CY1" s="37"/>
-      <c r="CZ1" s="37"/>
-      <c r="DA1" s="37"/>
-      <c r="DB1" s="37"/>
-      <c r="DC1" s="37"/>
-      <c r="DD1" s="37"/>
-      <c r="DE1" s="37"/>
-      <c r="DF1" s="37"/>
-      <c r="DG1" s="37"/>
-      <c r="DH1" s="37"/>
-      <c r="DI1" s="37"/>
-      <c r="DJ1" s="37"/>
-      <c r="DK1" s="37"/>
-      <c r="DL1" s="37"/>
-      <c r="DM1" s="37"/>
-      <c r="DN1" s="37"/>
-      <c r="DO1" s="37"/>
-      <c r="DP1" s="37"/>
-      <c r="DQ1" s="37"/>
-      <c r="DR1" s="37"/>
-      <c r="DS1" s="37"/>
-      <c r="DT1" s="37"/>
-      <c r="DU1" s="37"/>
-      <c r="DV1" s="37"/>
-      <c r="DW1" s="37"/>
-      <c r="DX1" s="37"/>
-      <c r="DY1" s="37"/>
-      <c r="DZ1" s="37"/>
-      <c r="EA1" s="37"/>
-      <c r="EB1" s="37"/>
-      <c r="EC1" s="37"/>
-      <c r="ED1" s="37"/>
-      <c r="EE1" s="37"/>
-      <c r="EF1" s="37"/>
-      <c r="EG1" s="37"/>
-      <c r="EH1" s="37"/>
-      <c r="EI1" s="37"/>
-      <c r="EJ1" s="37"/>
-      <c r="EK1" s="37"/>
-      <c r="EL1" s="37"/>
-      <c r="EM1" s="37"/>
-      <c r="EN1" s="37"/>
-      <c r="EO1" s="37"/>
-      <c r="EP1" s="37"/>
-      <c r="EQ1" s="37"/>
-      <c r="ER1" s="37"/>
-      <c r="ES1" s="37"/>
-      <c r="ET1" s="37"/>
-      <c r="EU1" s="37"/>
-      <c r="EV1" s="37"/>
-      <c r="EW1" s="37"/>
-      <c r="EX1" s="37"/>
-      <c r="EY1" s="37"/>
-      <c r="EZ1" s="37"/>
-      <c r="FA1" s="37"/>
-      <c r="FB1" s="37"/>
-      <c r="FC1" s="37"/>
-      <c r="FD1" s="37"/>
-      <c r="FE1" s="37"/>
-      <c r="FF1" s="37"/>
-      <c r="FG1" s="37"/>
-      <c r="FH1" s="37"/>
-      <c r="FI1" s="37"/>
-      <c r="FJ1" s="37"/>
-      <c r="FK1" s="37"/>
-      <c r="FL1" s="37"/>
-      <c r="FM1" s="37"/>
-      <c r="FN1" s="37"/>
-      <c r="FO1" s="37"/>
-      <c r="FP1" s="37"/>
-      <c r="FQ1" s="37"/>
-      <c r="FR1" s="37"/>
-      <c r="FS1" s="37"/>
-      <c r="FT1" s="37"/>
-      <c r="FU1" s="37"/>
-      <c r="FV1" s="37"/>
-      <c r="FW1" s="37"/>
-      <c r="FX1" s="37"/>
-      <c r="FY1" s="37"/>
-      <c r="FZ1" s="37"/>
-      <c r="GA1" s="37"/>
-      <c r="GB1" s="37"/>
-      <c r="GC1" s="37"/>
-      <c r="GD1" s="37"/>
-      <c r="GE1" s="37"/>
-      <c r="GF1" s="37"/>
-      <c r="GG1" s="37"/>
-      <c r="GH1" s="37"/>
-      <c r="GI1" s="37"/>
-      <c r="GJ1" s="37"/>
-      <c r="GK1" s="37"/>
-      <c r="GL1" s="37"/>
-      <c r="GM1" s="37"/>
-      <c r="GN1" s="37"/>
-      <c r="GO1" s="37"/>
-      <c r="GP1" s="37"/>
-      <c r="GQ1" s="37"/>
-      <c r="GR1" s="37"/>
-      <c r="GS1" s="37"/>
-      <c r="GT1" s="37"/>
-      <c r="GU1" s="37"/>
-      <c r="GV1" s="37"/>
-      <c r="GW1" s="37"/>
-      <c r="GX1" s="37"/>
-      <c r="GY1" s="37"/>
-      <c r="GZ1" s="37"/>
-      <c r="HA1" s="37"/>
-      <c r="HB1" s="37"/>
-      <c r="HC1" s="37"/>
-      <c r="HD1" s="37"/>
-      <c r="HE1" s="37"/>
-      <c r="HF1" s="37"/>
-      <c r="HG1" s="37"/>
-      <c r="HH1" s="37"/>
-      <c r="HI1" s="37"/>
-      <c r="HJ1" s="37"/>
-      <c r="HK1" s="37"/>
-      <c r="HL1" s="37"/>
-      <c r="HM1" s="37"/>
-      <c r="HN1" s="37"/>
-      <c r="HO1" s="37"/>
-      <c r="HP1" s="37"/>
-      <c r="HQ1" s="37"/>
-      <c r="HR1" s="37"/>
-      <c r="HS1" s="37"/>
-      <c r="HT1" s="37"/>
-      <c r="HU1" s="37"/>
-      <c r="HV1" s="37"/>
-      <c r="HW1" s="37"/>
-      <c r="HX1" s="37"/>
-      <c r="HY1" s="37"/>
-      <c r="HZ1" s="37"/>
-      <c r="IA1" s="37"/>
-      <c r="IB1" s="37"/>
-      <c r="IC1" s="37"/>
-      <c r="ID1" s="37"/>
-      <c r="IE1" s="37"/>
-      <c r="IF1" s="37"/>
-      <c r="IG1" s="37"/>
-      <c r="IH1" s="37"/>
-      <c r="II1" s="37"/>
-      <c r="IJ1" s="37"/>
-      <c r="IK1" s="37"/>
-      <c r="IL1" s="37"/>
-      <c r="IM1" s="37"/>
-      <c r="IN1" s="37"/>
-      <c r="IO1" s="37"/>
-      <c r="IP1" s="37"/>
-      <c r="IQ1" s="37"/>
-      <c r="IR1" s="37"/>
-      <c r="IS1" s="37"/>
-      <c r="IT1" s="37"/>
-      <c r="IU1" s="37"/>
-      <c r="IV1" s="37"/>
-      <c r="IW1" s="37"/>
-      <c r="IX1" s="37"/>
-      <c r="IY1" s="37"/>
-      <c r="IZ1" s="37"/>
-      <c r="JA1" s="37"/>
-      <c r="JB1" s="37"/>
-      <c r="JC1" s="37"/>
-      <c r="JD1" s="37"/>
-      <c r="JE1" s="37"/>
-      <c r="JF1" s="37"/>
-      <c r="JG1" s="37"/>
-      <c r="JH1" s="37"/>
-      <c r="JI1" s="37"/>
-      <c r="JJ1" s="37"/>
-      <c r="JK1" s="37"/>
-      <c r="JL1" s="37"/>
-      <c r="JM1" s="37"/>
-      <c r="JN1" s="37"/>
-      <c r="JO1" s="37"/>
-      <c r="JP1" s="37"/>
-      <c r="JQ1" s="37"/>
-      <c r="JR1" s="37"/>
-      <c r="JS1" s="37"/>
-      <c r="JT1" s="37"/>
-      <c r="JU1" s="37"/>
-      <c r="JV1" s="37"/>
-      <c r="JW1" s="37"/>
-      <c r="JX1" s="37"/>
-      <c r="JY1" s="37"/>
-      <c r="JZ1" s="37"/>
-      <c r="KA1" s="37"/>
-      <c r="KB1" s="37"/>
-      <c r="KC1" s="37"/>
-      <c r="KD1" s="37"/>
-      <c r="KE1" s="37"/>
-      <c r="KF1" s="37"/>
-      <c r="KG1" s="37"/>
-      <c r="KH1" s="37"/>
-      <c r="KI1" s="37"/>
-      <c r="KJ1" s="37"/>
-      <c r="KK1" s="37"/>
-      <c r="KL1" s="37"/>
-      <c r="KM1" s="37"/>
-      <c r="KN1" s="37"/>
-      <c r="KO1" s="37"/>
-      <c r="KP1" s="37"/>
-      <c r="KQ1" s="37"/>
-      <c r="KR1" s="37"/>
-      <c r="KS1" s="37"/>
-      <c r="KT1" s="37"/>
-      <c r="KU1" s="37"/>
-      <c r="KV1" s="37"/>
-      <c r="KW1" s="37"/>
-      <c r="KX1" s="37"/>
-      <c r="KY1" s="37"/>
-      <c r="KZ1" s="37"/>
-      <c r="LA1" s="37"/>
-      <c r="LB1" s="37"/>
-      <c r="LC1" s="37"/>
-      <c r="LD1" s="37"/>
-      <c r="LE1" s="37"/>
-      <c r="LF1" s="37"/>
-      <c r="LG1" s="37"/>
-      <c r="LH1" s="37"/>
-      <c r="LI1" s="37"/>
-      <c r="LJ1" s="37"/>
-      <c r="LK1" s="37"/>
-      <c r="LL1" s="37"/>
-      <c r="LM1" s="37"/>
-      <c r="LN1" s="37"/>
-      <c r="LO1" s="37"/>
-      <c r="LP1" s="37"/>
-      <c r="LQ1" s="37"/>
-      <c r="LR1" s="37"/>
-      <c r="LS1" s="37"/>
-      <c r="LT1" s="37"/>
-      <c r="LU1" s="37"/>
-      <c r="LV1" s="37"/>
-      <c r="LW1" s="37"/>
-      <c r="LX1" s="37"/>
-      <c r="LY1" s="37"/>
-      <c r="LZ1" s="37"/>
-      <c r="MA1" s="37"/>
-      <c r="MB1" s="37"/>
-      <c r="MC1" s="37"/>
-      <c r="MD1" s="37"/>
-      <c r="ME1" s="37"/>
-      <c r="MF1" s="37"/>
-      <c r="MG1" s="37"/>
-      <c r="MH1" s="37"/>
-      <c r="MI1" s="37"/>
-      <c r="MJ1" s="37"/>
-      <c r="MK1" s="37"/>
-      <c r="ML1" s="37"/>
-      <c r="MM1" s="37"/>
-      <c r="MN1" s="37"/>
-      <c r="MO1" s="37"/>
-      <c r="MP1" s="37"/>
-      <c r="MQ1" s="37"/>
-      <c r="MR1" s="37"/>
-      <c r="MS1" s="37"/>
-      <c r="MT1" s="37"/>
-      <c r="MU1" s="37"/>
-      <c r="MV1" s="37"/>
-      <c r="MW1" s="37"/>
-      <c r="MX1" s="37"/>
-      <c r="MY1" s="37"/>
-      <c r="MZ1" s="37"/>
-      <c r="NA1" s="37"/>
-      <c r="NB1" s="37"/>
-      <c r="NC1" s="37"/>
-      <c r="ND1" s="37"/>
-      <c r="NE1" s="37"/>
-      <c r="NF1" s="37"/>
-      <c r="NG1" s="37"/>
-      <c r="NH1" s="37"/>
-      <c r="NI1" s="37"/>
-      <c r="NJ1" s="37"/>
-      <c r="NK1" s="37"/>
-      <c r="NL1" s="37"/>
-      <c r="NM1" s="37"/>
-      <c r="NN1" s="37"/>
-      <c r="NO1" s="37"/>
-      <c r="NP1" s="37"/>
-      <c r="NQ1" s="37"/>
-      <c r="NR1" s="37"/>
-      <c r="NS1" s="37"/>
-      <c r="NT1" s="37"/>
-      <c r="NU1" s="37"/>
-      <c r="NV1" s="37"/>
-      <c r="NW1" s="37"/>
-      <c r="NX1" s="37"/>
-      <c r="NY1" s="37"/>
-      <c r="NZ1" s="37"/>
-      <c r="OA1" s="37"/>
-      <c r="OB1" s="37"/>
-      <c r="OC1" s="37"/>
-      <c r="OD1" s="37"/>
-      <c r="OE1" s="37"/>
-      <c r="OF1" s="37"/>
-      <c r="OG1" s="37"/>
-      <c r="OH1" s="37"/>
-      <c r="OI1" s="37"/>
-      <c r="OJ1" s="37"/>
-      <c r="OK1" s="37"/>
-      <c r="OL1" s="37"/>
-      <c r="OM1" s="37"/>
-      <c r="ON1" s="37"/>
-      <c r="OO1" s="37"/>
-      <c r="OP1" s="37"/>
-      <c r="OQ1" s="37"/>
-      <c r="OR1" s="37"/>
+      <c r="U1" s="30"/>
+      <c r="V1" s="31"/>
+      <c r="W1" s="31"/>
+      <c r="X1" s="31"/>
+      <c r="Y1" s="31"/>
+      <c r="Z1" s="31"/>
+      <c r="AA1" s="31"/>
+      <c r="AB1" s="31"/>
+      <c r="AC1" s="31"/>
+      <c r="AD1" s="31"/>
+      <c r="AE1" s="31"/>
+      <c r="AF1" s="31"/>
+      <c r="AG1" s="31"/>
+      <c r="AH1" s="31"/>
+      <c r="AI1" s="31"/>
+      <c r="AJ1" s="31"/>
+      <c r="AK1" s="31"/>
+      <c r="AL1" s="31"/>
+      <c r="AM1" s="31"/>
+      <c r="AN1" s="31"/>
+      <c r="AO1" s="31"/>
+      <c r="AP1" s="31"/>
+      <c r="AQ1" s="31"/>
+      <c r="AR1" s="31"/>
+      <c r="AS1" s="31"/>
+      <c r="AT1" s="31"/>
+      <c r="AU1" s="31"/>
+      <c r="AV1" s="31"/>
+      <c r="AW1" s="31"/>
+      <c r="AX1" s="31"/>
+      <c r="AY1" s="31"/>
+      <c r="AZ1" s="31"/>
+      <c r="BA1" s="31"/>
+      <c r="BB1" s="31"/>
+      <c r="BC1" s="31"/>
+      <c r="BD1" s="31"/>
+      <c r="BE1" s="31"/>
+      <c r="BF1" s="31"/>
+      <c r="BG1" s="31"/>
+      <c r="BH1" s="31"/>
+      <c r="BI1" s="31"/>
+      <c r="BJ1" s="31"/>
+      <c r="BK1" s="31"/>
+      <c r="BL1" s="31"/>
+      <c r="BM1" s="31"/>
+      <c r="BN1" s="31"/>
+      <c r="BO1" s="31"/>
+      <c r="BP1" s="31"/>
+      <c r="BQ1" s="31"/>
+      <c r="BR1" s="31"/>
+      <c r="BS1" s="31"/>
+      <c r="BT1" s="31"/>
+      <c r="BU1" s="31"/>
+      <c r="BV1" s="31"/>
+      <c r="BW1" s="31"/>
+      <c r="BX1" s="31"/>
+      <c r="BY1" s="31"/>
+      <c r="BZ1" s="31"/>
+      <c r="CA1" s="31"/>
+      <c r="CB1" s="31"/>
+      <c r="CC1" s="31"/>
+      <c r="CD1" s="31"/>
+      <c r="CE1" s="31"/>
+      <c r="CF1" s="31"/>
+      <c r="CG1" s="31"/>
+      <c r="CH1" s="31"/>
+      <c r="CI1" s="31"/>
+      <c r="CJ1" s="31"/>
+      <c r="CK1" s="31"/>
+      <c r="CL1" s="31"/>
+      <c r="CM1" s="31"/>
+      <c r="CN1" s="31"/>
+      <c r="CO1" s="31"/>
+      <c r="CP1" s="31"/>
+      <c r="CQ1" s="31"/>
+      <c r="CR1" s="31"/>
+      <c r="CS1" s="31"/>
+      <c r="CT1" s="31"/>
+      <c r="CU1" s="31"/>
+      <c r="CV1" s="31"/>
+      <c r="CW1" s="31"/>
+      <c r="CX1" s="31"/>
+      <c r="CY1" s="31"/>
+      <c r="CZ1" s="31"/>
+      <c r="DA1" s="31"/>
+      <c r="DB1" s="31"/>
+      <c r="DC1" s="31"/>
+      <c r="DD1" s="31"/>
+      <c r="DE1" s="31"/>
+      <c r="DF1" s="31"/>
+      <c r="DG1" s="31"/>
+      <c r="DH1" s="31"/>
+      <c r="DI1" s="31"/>
+      <c r="DJ1" s="31"/>
+      <c r="DK1" s="31"/>
+      <c r="DL1" s="31"/>
+      <c r="DM1" s="31"/>
+      <c r="DN1" s="31"/>
+      <c r="DO1" s="31"/>
+      <c r="DP1" s="31"/>
+      <c r="DQ1" s="31"/>
+      <c r="DR1" s="31"/>
+      <c r="DS1" s="31"/>
+      <c r="DT1" s="31"/>
+      <c r="DU1" s="31"/>
+      <c r="DV1" s="31"/>
+      <c r="DW1" s="31"/>
+      <c r="DX1" s="31"/>
+      <c r="DY1" s="31"/>
+      <c r="DZ1" s="31"/>
+      <c r="EA1" s="31"/>
+      <c r="EB1" s="31"/>
+      <c r="EC1" s="31"/>
+      <c r="ED1" s="31"/>
+      <c r="EE1" s="31"/>
+      <c r="EF1" s="31"/>
+      <c r="EG1" s="31"/>
+      <c r="EH1" s="31"/>
+      <c r="EI1" s="31"/>
+      <c r="EJ1" s="31"/>
+      <c r="EK1" s="31"/>
+      <c r="EL1" s="31"/>
+      <c r="EM1" s="31"/>
+      <c r="EN1" s="31"/>
+      <c r="EO1" s="31"/>
+      <c r="EP1" s="31"/>
+      <c r="EQ1" s="31"/>
+      <c r="ER1" s="31"/>
+      <c r="ES1" s="31"/>
+      <c r="ET1" s="31"/>
+      <c r="EU1" s="31"/>
+      <c r="EV1" s="31"/>
+      <c r="EW1" s="31"/>
+      <c r="EX1" s="31"/>
+      <c r="EY1" s="31"/>
+      <c r="EZ1" s="31"/>
+      <c r="FA1" s="31"/>
+      <c r="FB1" s="31"/>
+      <c r="FC1" s="31"/>
+      <c r="FD1" s="31"/>
+      <c r="FE1" s="31"/>
+      <c r="FF1" s="31"/>
+      <c r="FG1" s="31"/>
+      <c r="FH1" s="31"/>
+      <c r="FI1" s="31"/>
+      <c r="FJ1" s="31"/>
+      <c r="FK1" s="31"/>
+      <c r="FL1" s="31"/>
+      <c r="FM1" s="31"/>
+      <c r="FN1" s="31"/>
+      <c r="FO1" s="31"/>
+      <c r="FP1" s="31"/>
+      <c r="FQ1" s="31"/>
+      <c r="FR1" s="31"/>
+      <c r="FS1" s="31"/>
+      <c r="FT1" s="31"/>
+      <c r="FU1" s="31"/>
+      <c r="FV1" s="31"/>
+      <c r="FW1" s="31"/>
+      <c r="FX1" s="31"/>
+      <c r="FY1" s="31"/>
+      <c r="FZ1" s="31"/>
+      <c r="GA1" s="31"/>
+      <c r="GB1" s="31"/>
+      <c r="GC1" s="31"/>
+      <c r="GD1" s="31"/>
+      <c r="GE1" s="31"/>
+      <c r="GF1" s="31"/>
+      <c r="GG1" s="31"/>
+      <c r="GH1" s="31"/>
+      <c r="GI1" s="31"/>
+      <c r="GJ1" s="31"/>
+      <c r="GK1" s="31"/>
+      <c r="GL1" s="31"/>
+      <c r="GM1" s="31"/>
+      <c r="GN1" s="31"/>
+      <c r="GO1" s="31"/>
+      <c r="GP1" s="31"/>
+      <c r="GQ1" s="31"/>
+      <c r="GR1" s="31"/>
+      <c r="GS1" s="31"/>
+      <c r="GT1" s="31"/>
+      <c r="GU1" s="31"/>
+      <c r="GV1" s="31"/>
+      <c r="GW1" s="31"/>
+      <c r="GX1" s="31"/>
+      <c r="GY1" s="31"/>
+      <c r="GZ1" s="31"/>
+      <c r="HA1" s="31"/>
+      <c r="HB1" s="31"/>
+      <c r="HC1" s="31"/>
+      <c r="HD1" s="31"/>
+      <c r="HE1" s="31"/>
+      <c r="HF1" s="31"/>
+      <c r="HG1" s="31"/>
+      <c r="HH1" s="31"/>
+      <c r="HI1" s="31"/>
+      <c r="HJ1" s="31"/>
+      <c r="HK1" s="31"/>
+      <c r="HL1" s="31"/>
+      <c r="HM1" s="31"/>
+      <c r="HN1" s="31"/>
+      <c r="HO1" s="31"/>
+      <c r="HP1" s="31"/>
+      <c r="HQ1" s="31"/>
+      <c r="HR1" s="31"/>
+      <c r="HS1" s="31"/>
+      <c r="HT1" s="31"/>
+      <c r="HU1" s="31"/>
+      <c r="HV1" s="31"/>
+      <c r="HW1" s="31"/>
+      <c r="HX1" s="31"/>
+      <c r="HY1" s="31"/>
+      <c r="HZ1" s="31"/>
+      <c r="IA1" s="31"/>
+      <c r="IB1" s="31"/>
+      <c r="IC1" s="31"/>
+      <c r="ID1" s="31"/>
+      <c r="IE1" s="31"/>
+      <c r="IF1" s="31"/>
+      <c r="IG1" s="31"/>
+      <c r="IH1" s="31"/>
+      <c r="II1" s="31"/>
+      <c r="IJ1" s="31"/>
+      <c r="IK1" s="31"/>
+      <c r="IL1" s="31"/>
+      <c r="IM1" s="31"/>
+      <c r="IN1" s="31"/>
+      <c r="IO1" s="31"/>
+      <c r="IP1" s="31"/>
+      <c r="IQ1" s="31"/>
+      <c r="IR1" s="31"/>
+      <c r="IS1" s="31"/>
+      <c r="IT1" s="31"/>
+      <c r="IU1" s="31"/>
+      <c r="IV1" s="31"/>
+      <c r="IW1" s="31"/>
+      <c r="IX1" s="31"/>
+      <c r="IY1" s="31"/>
+      <c r="IZ1" s="31"/>
+      <c r="JA1" s="31"/>
+      <c r="JB1" s="31"/>
+      <c r="JC1" s="31"/>
+      <c r="JD1" s="31"/>
+      <c r="JE1" s="31"/>
+      <c r="JF1" s="31"/>
+      <c r="JG1" s="31"/>
+      <c r="JH1" s="31"/>
+      <c r="JI1" s="31"/>
+      <c r="JJ1" s="31"/>
+      <c r="JK1" s="31"/>
+      <c r="JL1" s="31"/>
+      <c r="JM1" s="31"/>
+      <c r="JN1" s="31"/>
+      <c r="JO1" s="31"/>
+      <c r="JP1" s="31"/>
+      <c r="JQ1" s="31"/>
+      <c r="JR1" s="31"/>
+      <c r="JS1" s="31"/>
+      <c r="JT1" s="31"/>
+      <c r="JU1" s="31"/>
+      <c r="JV1" s="31"/>
+      <c r="JW1" s="31"/>
+      <c r="JX1" s="31"/>
+      <c r="JY1" s="31"/>
+      <c r="JZ1" s="31"/>
+      <c r="KA1" s="31"/>
+      <c r="KB1" s="31"/>
+      <c r="KC1" s="31"/>
+      <c r="KD1" s="31"/>
+      <c r="KE1" s="31"/>
+      <c r="KF1" s="31"/>
+      <c r="KG1" s="31"/>
+      <c r="KH1" s="31"/>
+      <c r="KI1" s="31"/>
+      <c r="KJ1" s="31"/>
+      <c r="KK1" s="31"/>
+      <c r="KL1" s="31"/>
+      <c r="KM1" s="31"/>
+      <c r="KN1" s="31"/>
+      <c r="KO1" s="31"/>
+      <c r="KP1" s="31"/>
+      <c r="KQ1" s="31"/>
+      <c r="KR1" s="31"/>
+      <c r="KS1" s="31"/>
+      <c r="KT1" s="31"/>
+      <c r="KU1" s="31"/>
+      <c r="KV1" s="31"/>
+      <c r="KW1" s="31"/>
+      <c r="KX1" s="31"/>
+      <c r="KY1" s="31"/>
+      <c r="KZ1" s="31"/>
+      <c r="LA1" s="31"/>
+      <c r="LB1" s="31"/>
+      <c r="LC1" s="31"/>
+      <c r="LD1" s="31"/>
+      <c r="LE1" s="31"/>
+      <c r="LF1" s="31"/>
+      <c r="LG1" s="31"/>
+      <c r="LH1" s="31"/>
+      <c r="LI1" s="31"/>
+      <c r="LJ1" s="31"/>
+      <c r="LK1" s="31"/>
+      <c r="LL1" s="31"/>
+      <c r="LM1" s="31"/>
+      <c r="LN1" s="31"/>
+      <c r="LO1" s="31"/>
+      <c r="LP1" s="31"/>
+      <c r="LQ1" s="31"/>
+      <c r="LR1" s="31"/>
+      <c r="LS1" s="31"/>
+      <c r="LT1" s="31"/>
+      <c r="LU1" s="31"/>
+      <c r="LV1" s="31"/>
+      <c r="LW1" s="31"/>
+      <c r="LX1" s="31"/>
+      <c r="LY1" s="31"/>
+      <c r="LZ1" s="31"/>
+      <c r="MA1" s="31"/>
+      <c r="MB1" s="31"/>
+      <c r="MC1" s="31"/>
+      <c r="MD1" s="31"/>
+      <c r="ME1" s="31"/>
+      <c r="MF1" s="31"/>
+      <c r="MG1" s="31"/>
+      <c r="MH1" s="31"/>
+      <c r="MI1" s="31"/>
+      <c r="MJ1" s="31"/>
+      <c r="MK1" s="31"/>
+      <c r="ML1" s="31"/>
+      <c r="MM1" s="31"/>
+      <c r="MN1" s="31"/>
+      <c r="MO1" s="31"/>
+      <c r="MP1" s="31"/>
+      <c r="MQ1" s="31"/>
+      <c r="MR1" s="31"/>
+      <c r="MS1" s="31"/>
+      <c r="MT1" s="31"/>
+      <c r="MU1" s="31"/>
+      <c r="MV1" s="31"/>
+      <c r="MW1" s="31"/>
+      <c r="MX1" s="31"/>
+      <c r="MY1" s="31"/>
+      <c r="MZ1" s="31"/>
+      <c r="NA1" s="31"/>
+      <c r="NB1" s="31"/>
+      <c r="NC1" s="31"/>
+      <c r="ND1" s="31"/>
+      <c r="NE1" s="31"/>
+      <c r="NF1" s="31"/>
+      <c r="NG1" s="31"/>
+      <c r="NH1" s="31"/>
+      <c r="NI1" s="31"/>
+      <c r="NJ1" s="31"/>
+      <c r="NK1" s="31"/>
+      <c r="NL1" s="31"/>
+      <c r="NM1" s="31"/>
+      <c r="NN1" s="31"/>
+      <c r="NO1" s="31"/>
+      <c r="NP1" s="31"/>
+      <c r="NQ1" s="31"/>
+      <c r="NR1" s="31"/>
+      <c r="NS1" s="31"/>
+      <c r="NT1" s="31"/>
+      <c r="NU1" s="31"/>
+      <c r="NV1" s="31"/>
+      <c r="NW1" s="31"/>
+      <c r="NX1" s="31"/>
+      <c r="NY1" s="31"/>
+      <c r="NZ1" s="31"/>
+      <c r="OA1" s="31"/>
+      <c r="OB1" s="31"/>
+      <c r="OC1" s="31"/>
+      <c r="OD1" s="31"/>
+      <c r="OE1" s="31"/>
+      <c r="OF1" s="31"/>
+      <c r="OG1" s="31"/>
+      <c r="OH1" s="31"/>
+      <c r="OI1" s="31"/>
+      <c r="OJ1" s="31"/>
+      <c r="OK1" s="31"/>
+      <c r="OL1" s="31"/>
+      <c r="OM1" s="31"/>
+      <c r="ON1" s="31"/>
+      <c r="OO1" s="31"/>
+      <c r="OP1" s="31"/>
+      <c r="OQ1" s="31"/>
+      <c r="OR1" s="31"/>
     </row>
-    <row r="2" ht="15.7" spans="1:21">
+    <row r="2" ht="13.5" spans="1:21">
       <c r="A2" s="10"/>
       <c r="B2" s="11"/>
       <c r="C2" s="12"/>
@@ -2653,7 +2638,7 @@
       <c r="R2" s="11"/>
       <c r="S2" s="12"/>
       <c r="T2" s="11"/>
-      <c r="U2" s="38"/>
+      <c r="U2" s="32"/>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" s="3" t="s">
@@ -2680,7 +2665,7 @@
       <c r="J3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K3" s="41" t="s">
+      <c r="K3" s="35" t="s">
         <v>28</v>
       </c>
       <c r="L3" s="4" t="s">
@@ -2910,7 +2895,7 @@
       <c r="K7" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="L7" s="31" t="s">
+      <c r="L7" s="4" t="s">
         <v>48</v>
       </c>
       <c r="M7" s="5">
@@ -3022,7 +3007,7 @@
       <c r="K9" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="L9" s="31" t="s">
+      <c r="L9" s="4" t="s">
         <v>56</v>
       </c>
       <c r="M9" s="5">
@@ -3066,20 +3051,20 @@
       <c r="D10" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E10" s="25"/>
+      <c r="E10" s="22"/>
       <c r="F10" s="4" t="s">
         <v>25</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="J10" s="32" t="s">
+      <c r="J10" s="26" t="s">
         <v>59</v>
       </c>
       <c r="K10" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="L10" s="31" t="s">
+      <c r="L10" s="4" t="s">
         <v>61</v>
       </c>
       <c r="M10" s="5">
@@ -3123,14 +3108,14 @@
       <c r="D11" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="E11" s="25"/>
+      <c r="E11" s="22"/>
       <c r="F11" s="4" t="s">
         <v>25</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="J11" s="32" t="s">
+      <c r="J11" s="26" t="s">
         <v>59</v>
       </c>
       <c r="K11" s="5" t="s">
@@ -3292,14 +3277,14 @@
       <c r="D14" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="E14" s="25"/>
+      <c r="E14" s="22"/>
       <c r="F14" s="4" t="s">
         <v>25</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="J14" s="32" t="s">
+      <c r="J14" s="26" t="s">
         <v>59</v>
       </c>
       <c r="K14" s="5" t="s">
@@ -3413,7 +3398,7 @@
       <c r="R16" s="11"/>
       <c r="S16" s="16"/>
       <c r="T16" s="15"/>
-      <c r="U16" s="39"/>
+      <c r="U16" s="33"/>
     </row>
     <row r="17" s="2" customFormat="1" spans="1:408">
       <c r="A17" s="14"/>
@@ -3436,7 +3421,7 @@
       <c r="R17" s="11"/>
       <c r="S17" s="16"/>
       <c r="T17" s="15"/>
-      <c r="U17" s="39"/>
+      <c r="U17" s="33"/>
       <c r="V17" s="7"/>
       <c r="W17" s="7"/>
       <c r="X17" s="7"/>
@@ -3906,7 +3891,7 @@
       <c r="R19" s="11"/>
       <c r="S19" s="16"/>
       <c r="T19" s="15"/>
-      <c r="U19" s="39"/>
+      <c r="U19" s="33"/>
       <c r="V19" s="7"/>
       <c r="W19" s="7"/>
       <c r="X19" s="7"/>
@@ -4424,7 +4409,7 @@
       <c r="R22" s="11"/>
       <c r="S22" s="16"/>
       <c r="T22" s="15"/>
-      <c r="U22" s="39"/>
+      <c r="U22" s="33"/>
       <c r="V22" s="7"/>
       <c r="W22" s="7"/>
       <c r="X22" s="7"/>
@@ -4862,10 +4847,9 @@
       <c r="Q23" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="R23" s="4"/>
       <c r="S23" s="19"/>
       <c r="T23" s="20"/>
-      <c r="U23" s="40"/>
+      <c r="U23" s="34"/>
     </row>
     <row r="24" s="2" customFormat="1" spans="1:408">
       <c r="A24" s="14"/>
@@ -4888,7 +4872,7 @@
       <c r="R24" s="11"/>
       <c r="S24" s="16"/>
       <c r="T24" s="15"/>
-      <c r="U24" s="39"/>
+      <c r="U24" s="33"/>
       <c r="V24" s="7"/>
       <c r="W24" s="7"/>
       <c r="X24" s="7"/>
@@ -5305,7 +5289,7 @@
       <c r="K25" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="L25" s="31" t="s">
+      <c r="L25" s="27" t="s">
         <v>114</v>
       </c>
       <c r="M25" s="5">
@@ -5353,7 +5337,7 @@
       <c r="E26" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="F26" s="26" t="s">
+      <c r="F26" s="23" t="s">
         <v>118</v>
       </c>
       <c r="G26" s="5" t="s">
@@ -5365,7 +5349,7 @@
       <c r="K26" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="L26" s="31" t="s">
+      <c r="L26" s="27" t="s">
         <v>120</v>
       </c>
       <c r="M26" s="5">
@@ -5413,7 +5397,7 @@
       <c r="E27" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="F27" s="26" t="s">
+      <c r="F27" s="23" t="s">
         <v>118</v>
       </c>
       <c r="G27" s="5" t="s">
@@ -5425,7 +5409,7 @@
       <c r="K27" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="L27" s="31" t="s">
+      <c r="L27" s="27" t="s">
         <v>124</v>
       </c>
       <c r="M27" s="5">
@@ -5485,7 +5469,7 @@
       <c r="K28" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="L28" s="4" t="s">
+      <c r="L28" s="27" t="s">
         <v>129</v>
       </c>
       <c r="M28" s="5">
@@ -5542,7 +5526,7 @@
       <c r="K29" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="L29" s="4" t="s">
+      <c r="L29" s="27" t="s">
         <v>134</v>
       </c>
       <c r="M29" s="5">
@@ -5586,7 +5570,7 @@
       <c r="I30" s="16"/>
       <c r="J30" s="15"/>
       <c r="K30" s="16"/>
-      <c r="L30" s="15"/>
+      <c r="L30" s="27"/>
       <c r="M30" s="16"/>
       <c r="N30" s="15"/>
       <c r="O30" s="16"/>
@@ -5595,7 +5579,7 @@
       <c r="R30" s="11"/>
       <c r="S30" s="16"/>
       <c r="T30" s="15"/>
-      <c r="U30" s="39"/>
+      <c r="U30" s="33"/>
       <c r="V30" s="7"/>
       <c r="W30" s="7"/>
       <c r="X30" s="7"/>
@@ -5997,7 +5981,7 @@
       <c r="D31" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="E31" s="23" t="s">
+      <c r="E31" s="5" t="s">
         <v>139</v>
       </c>
       <c r="F31" s="4" t="s">
@@ -6012,7 +5996,7 @@
       <c r="K31" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="L31" s="4" t="s">
+      <c r="L31" s="27" t="s">
         <v>142</v>
       </c>
       <c r="M31" s="5">
@@ -6056,7 +6040,7 @@
       <c r="I32" s="16"/>
       <c r="J32" s="15"/>
       <c r="K32" s="16"/>
-      <c r="L32" s="15"/>
+      <c r="L32" s="27"/>
       <c r="M32" s="16"/>
       <c r="N32" s="15"/>
       <c r="O32" s="16"/>
@@ -6065,7 +6049,7 @@
       <c r="R32" s="11"/>
       <c r="S32" s="16"/>
       <c r="T32" s="15"/>
-      <c r="U32" s="39"/>
+      <c r="U32" s="33"/>
     </row>
     <row r="33" s="2" customFormat="1" spans="1:408">
       <c r="A33" s="14"/>
@@ -6079,7 +6063,7 @@
       <c r="I33" s="16"/>
       <c r="J33" s="15"/>
       <c r="K33" s="16"/>
-      <c r="L33" s="15"/>
+      <c r="L33" s="27"/>
       <c r="M33" s="16"/>
       <c r="N33" s="15"/>
       <c r="O33" s="16"/>
@@ -6088,7 +6072,7 @@
       <c r="R33" s="11"/>
       <c r="S33" s="16"/>
       <c r="T33" s="15"/>
-      <c r="U33" s="39"/>
+      <c r="U33" s="33"/>
       <c r="V33" s="7"/>
       <c r="W33" s="7"/>
       <c r="X33" s="7"/>
@@ -6493,7 +6477,7 @@
       <c r="E34" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="F34" s="27" t="s">
+      <c r="F34" s="23" t="s">
         <v>147</v>
       </c>
       <c r="G34" s="5" t="s">
@@ -6505,7 +6489,7 @@
       <c r="K34" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="L34" s="4" t="s">
+      <c r="L34" s="27" t="s">
         <v>149</v>
       </c>
       <c r="M34" s="5">
@@ -6549,7 +6533,7 @@
       <c r="I35" s="16"/>
       <c r="J35" s="15"/>
       <c r="K35" s="16"/>
-      <c r="L35" s="15"/>
+      <c r="L35" s="27"/>
       <c r="M35" s="16"/>
       <c r="N35" s="15"/>
       <c r="O35" s="16"/>
@@ -6558,7 +6542,7 @@
       <c r="R35" s="11"/>
       <c r="S35" s="16"/>
       <c r="T35" s="15"/>
-      <c r="U35" s="39"/>
+      <c r="U35" s="33"/>
       <c r="V35" s="7"/>
       <c r="W35" s="7"/>
       <c r="X35" s="7"/>
@@ -6960,7 +6944,7 @@
       <c r="D36" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="E36" s="28">
+      <c r="E36" s="24">
         <v>0.05</v>
       </c>
       <c r="F36" s="4" t="s">
@@ -6975,7 +6959,7 @@
       <c r="K36" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="L36" s="31" t="s">
+      <c r="L36" s="27" t="s">
         <v>154</v>
       </c>
       <c r="M36" s="5">
@@ -7034,7 +7018,7 @@
       <c r="K37" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="L37" s="4" t="s">
+      <c r="L37" s="27" t="s">
         <v>159</v>
       </c>
       <c r="M37" s="5">
@@ -7078,7 +7062,7 @@
       <c r="D38" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="E38" s="28">
+      <c r="E38" s="24">
         <v>0.05</v>
       </c>
       <c r="F38" s="4" t="s">
@@ -7093,7 +7077,7 @@
       <c r="K38" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="L38" s="4" t="s">
+      <c r="L38" s="27" t="s">
         <v>163</v>
       </c>
       <c r="M38" s="5">
@@ -7152,7 +7136,7 @@
       <c r="K39" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="L39" s="4" t="s">
+      <c r="L39" s="27" t="s">
         <v>168</v>
       </c>
       <c r="M39" s="5">
@@ -7196,7 +7180,7 @@
       <c r="D40" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="E40" s="28">
+      <c r="E40" s="24">
         <v>0.01</v>
       </c>
       <c r="F40" s="4" t="s">
@@ -7211,7 +7195,7 @@
       <c r="K40" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="L40" s="31" t="s">
+      <c r="L40" s="27" t="s">
         <v>171</v>
       </c>
       <c r="M40" s="5">
@@ -7255,7 +7239,7 @@
       <c r="D41" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="E41" s="28">
+      <c r="E41" s="24">
         <v>0.01</v>
       </c>
       <c r="F41" s="4" t="s">
@@ -7270,7 +7254,7 @@
       <c r="K41" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="L41" s="31" t="s">
+      <c r="L41" s="27" t="s">
         <v>175</v>
       </c>
       <c r="M41" s="5">
@@ -7314,7 +7298,7 @@
       <c r="D42" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="E42" s="28">
+      <c r="E42" s="24">
         <v>0.01</v>
       </c>
       <c r="F42" s="4" t="s">
@@ -7329,7 +7313,7 @@
       <c r="K42" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="L42" s="31" t="s">
+      <c r="L42" s="27" t="s">
         <v>179</v>
       </c>
       <c r="M42" s="5">
@@ -7373,7 +7357,7 @@
       <c r="D43" s="4" t="s">
         <v>181</v>
       </c>
-      <c r="E43" s="28">
+      <c r="E43" s="24">
         <v>0.01</v>
       </c>
       <c r="F43" s="4" t="s">
@@ -7388,7 +7372,7 @@
       <c r="K43" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="L43" s="31" t="s">
+      <c r="L43" s="27" t="s">
         <v>183</v>
       </c>
       <c r="M43" s="5">
@@ -7432,7 +7416,7 @@
       <c r="D44" s="4" t="s">
         <v>185</v>
       </c>
-      <c r="E44" s="28">
+      <c r="E44" s="24">
         <v>0.05</v>
       </c>
       <c r="F44" s="4" t="s">
@@ -7447,7 +7431,7 @@
       <c r="K44" s="5" t="s">
         <v>186</v>
       </c>
-      <c r="L44" s="4" t="s">
+      <c r="L44" s="27" t="s">
         <v>187</v>
       </c>
       <c r="M44" s="5">
@@ -7491,7 +7475,7 @@
       <c r="D45" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="E45" s="28">
+      <c r="E45" s="24">
         <v>0.01</v>
       </c>
       <c r="F45" s="4" t="s">
@@ -7503,10 +7487,10 @@
       <c r="J45" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="K45" s="33" t="s">
+      <c r="K45" s="28" t="s">
         <v>190</v>
       </c>
-      <c r="L45" s="4" t="s">
+      <c r="L45" s="27" t="s">
         <v>191</v>
       </c>
       <c r="M45" s="5">
@@ -7550,7 +7534,7 @@
       <c r="D46" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="E46" s="28">
+      <c r="E46" s="24">
         <v>0.01</v>
       </c>
       <c r="F46" s="4" t="s">
@@ -7565,7 +7549,7 @@
       <c r="K46" s="5" t="s">
         <v>194</v>
       </c>
-      <c r="L46" s="31" t="s">
+      <c r="L46" s="27" t="s">
         <v>195</v>
       </c>
       <c r="M46" s="5">
@@ -7609,7 +7593,7 @@
       <c r="D47" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="E47" s="28">
+      <c r="E47" s="24">
         <v>0.01</v>
       </c>
       <c r="F47" s="4" t="s">
@@ -7624,7 +7608,7 @@
       <c r="K47" s="5" t="s">
         <v>198</v>
       </c>
-      <c r="L47" s="31" t="s">
+      <c r="L47" s="27" t="s">
         <v>199</v>
       </c>
       <c r="M47" s="5">
@@ -7668,7 +7652,7 @@
       <c r="D48" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="E48" s="28">
+      <c r="E48" s="24">
         <v>0.01</v>
       </c>
       <c r="F48" s="4" t="s">
@@ -7683,7 +7667,7 @@
       <c r="K48" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="L48" s="4" t="s">
+      <c r="L48" s="27" t="s">
         <v>203</v>
       </c>
       <c r="M48" s="5">
@@ -7727,7 +7711,7 @@
       <c r="D49" s="4" t="s">
         <v>205</v>
       </c>
-      <c r="E49" s="28">
+      <c r="E49" s="24">
         <v>0.01</v>
       </c>
       <c r="F49" s="4" t="s">
@@ -7742,7 +7726,7 @@
       <c r="K49" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="L49" s="4" t="s">
+      <c r="L49" s="27" t="s">
         <v>207</v>
       </c>
       <c r="M49" s="5">
@@ -7786,7 +7770,7 @@
       <c r="D50" s="4" t="s">
         <v>209</v>
       </c>
-      <c r="E50" s="28" t="s">
+      <c r="E50" s="24" t="s">
         <v>210</v>
       </c>
       <c r="F50" s="4" t="s">
@@ -7801,7 +7785,7 @@
       <c r="K50" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="L50" s="31" t="s">
+      <c r="L50" s="27" t="s">
         <v>212</v>
       </c>
       <c r="M50" s="5">
@@ -7845,7 +7829,7 @@
       <c r="D51" s="4" t="s">
         <v>214</v>
       </c>
-      <c r="E51" s="28">
+      <c r="E51" s="24">
         <v>0.01</v>
       </c>
       <c r="F51" s="4" t="s">
@@ -7912,7 +7896,7 @@
       <c r="R52" s="11"/>
       <c r="S52" s="16"/>
       <c r="T52" s="15"/>
-      <c r="U52" s="39"/>
+      <c r="U52" s="33"/>
       <c r="V52" s="7"/>
       <c r="W52" s="7"/>
       <c r="X52" s="7"/>
@@ -8764,115 +8748,122 @@
       </c>
     </row>
     <row r="61" spans="1:21">
-      <c r="A61" s="21" t="s">
+      <c r="A61" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="B61" s="22" t="s">
+      <c r="B61" s="21" t="s">
         <v>272</v>
       </c>
-      <c r="C61" s="23" t="s">
+      <c r="C61" s="5" t="s">
         <v>228</v>
       </c>
-      <c r="D61" s="20" t="s">
+      <c r="D61" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="E61" s="29" t="s">
+      <c r="E61" s="25"/>
+      <c r="F61" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="F61" s="30" t="s">
+      <c r="G61" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="H61" s="4"/>
+      <c r="I61" s="5"/>
+      <c r="J61" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K61" s="29" t="s">
         <v>275</v>
       </c>
-      <c r="G61" s="19" t="s">
-        <v>223</v>
-      </c>
-      <c r="H61" s="20"/>
-      <c r="I61" s="19"/>
-      <c r="J61" s="32" t="s">
-        <v>274</v>
-      </c>
-      <c r="K61" s="23" t="s">
+      <c r="L61" s="27" t="s">
         <v>276</v>
       </c>
-      <c r="L61" s="30" t="s">
-        <v>277</v>
-      </c>
-      <c r="M61" s="23">
+      <c r="M61" s="29">
         <v>1</v>
       </c>
-      <c r="N61" s="30">
+      <c r="N61" s="27">
         <f t="shared" si="10"/>
         <v>3</v>
       </c>
-      <c r="O61" s="23">
-        <v>2.01</v>
-      </c>
-      <c r="P61" s="30">
-        <v>1.98</v>
-      </c>
-      <c r="Q61" s="23">
-        <v>1.53</v>
-      </c>
-      <c r="R61" s="34">
+      <c r="O61" s="29">
+        <v>1.94</v>
+      </c>
+      <c r="P61" s="27">
+        <v>1.91</v>
+      </c>
+      <c r="Q61" s="29">
+        <v>1.47</v>
+      </c>
+      <c r="R61" s="27">
         <f t="shared" si="7"/>
-        <v>2.01</v>
-      </c>
-      <c r="S61" s="35">
+        <v>1.94</v>
+      </c>
+      <c r="S61" s="29">
         <f t="shared" si="11"/>
-        <v>1.53</v>
-      </c>
-      <c r="T61" s="34">
+        <v>1.47</v>
+      </c>
+      <c r="T61" s="27">
         <f t="shared" si="12"/>
-        <v>6.03</v>
-      </c>
-      <c r="U61" s="40"/>
+        <v>5.82</v>
+      </c>
+      <c r="U61" s="34"/>
     </row>
     <row r="62" spans="1:21">
-      <c r="A62" s="17" t="s">
+      <c r="A62" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="B62" s="21" t="s">
         <v>278</v>
       </c>
-      <c r="B62" s="18" t="s">
+      <c r="C62" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="C62" s="24" t="s">
+      <c r="D62" s="4"/>
+      <c r="E62" s="19"/>
+      <c r="F62" s="4" t="s">
         <v>280</v>
       </c>
-      <c r="D62" s="20"/>
-      <c r="E62" s="19"/>
-      <c r="F62" s="20" t="s">
+      <c r="G62" s="5"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="5"/>
+      <c r="J62" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="K62" s="5" t="s">
         <v>281</v>
       </c>
-      <c r="G62" s="19"/>
-      <c r="H62" s="20"/>
-      <c r="I62" s="19"/>
-      <c r="J62" s="20" t="s">
-        <v>281</v>
-      </c>
-      <c r="K62" s="19" t="s">
-        <v>281</v>
-      </c>
-      <c r="L62" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="M62" s="19">
+      <c r="L62" s="27" t="s">
+        <v>282</v>
+      </c>
+      <c r="M62" s="29">
         <v>1</v>
       </c>
-      <c r="N62" s="20">
+      <c r="N62" s="27">
         <f t="shared" si="10"/>
         <v>3</v>
       </c>
-      <c r="O62" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="P62" s="20" t="s">
-        <v>105</v>
-      </c>
-      <c r="Q62" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="R62" s="4"/>
-      <c r="S62" s="5"/>
-      <c r="T62" s="20"/>
-      <c r="U62" s="40"/>
+      <c r="O62" s="29">
+        <v>0.367</v>
+      </c>
+      <c r="P62" s="27">
+        <v>0.362</v>
+      </c>
+      <c r="Q62" s="29">
+        <v>0.298</v>
+      </c>
+      <c r="R62" s="27">
+        <f>M62*O62</f>
+        <v>0.367</v>
+      </c>
+      <c r="S62" s="29">
+        <f>M62*Q62</f>
+        <v>0.298</v>
+      </c>
+      <c r="T62" s="27">
+        <f>N62*O62</f>
+        <v>1.101</v>
+      </c>
+      <c r="U62" s="34"/>
     </row>
     <row r="63" s="2" customFormat="1" spans="1:408">
       <c r="A63" s="14"/>
@@ -8895,7 +8886,7 @@
       <c r="R63" s="11"/>
       <c r="S63" s="16"/>
       <c r="T63" s="15"/>
-      <c r="U63" s="39"/>
+      <c r="U63" s="33"/>
       <c r="V63" s="7"/>
       <c r="W63" s="7"/>
       <c r="X63" s="7"/>
@@ -9286,32 +9277,32 @@
     </row>
     <row r="66" spans="18:20">
       <c r="R66" s="4" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="S66" s="5" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="T66" s="4" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
     </row>
     <row r="67" spans="18:20">
       <c r="R67" s="4">
         <f>SUM(R3:R63)</f>
-        <v>39.878</v>
+        <v>40.175</v>
       </c>
       <c r="S67" s="5">
         <f>SUM(S3:S62)</f>
-        <v>22.381</v>
+        <v>22.619</v>
       </c>
       <c r="T67" s="4">
         <f>SUM(T3:T63)</f>
-        <v>100.615</v>
+        <v>101.506</v>
       </c>
     </row>
     <row r="70" spans="4:7">
       <c r="D70" s="4" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="G70" s="5" t="s">
         <v>223</v>
@@ -9345,6 +9336,7 @@
     <hyperlink ref="L46" r:id="rId24" display="https://eu.mouser.com/ProductDetail/Yageo/RC0402FR-073K4L?qs=sGAEpiMZZMvdGkrng054t8AJgcdMkx7xgpEjmeLAGq8%3D"/>
     <hyperlink ref="L47" r:id="rId25" display="https://eu.mouser.com/ProductDetail/Yageo/RC0402FR-07301KL?qs=sGAEpiMZZMvdGkrng054tzwoVKV%2F7vUjLTxmZ0rOfsI%3D"/>
     <hyperlink ref="L50" r:id="rId26" display="https://eu.mouser.com/ProductDetail/Yageo/RC0402JR-074K7L?qs=sGAEpiMZZMvdGkrng054t3pr%252BPE%2FADjskcKxWeJKz3s%3D"/>
+    <hyperlink ref="L62" r:id="rId27" display="https://eu.mouser.com/ProductDetail/Winbond/W25Q80DVSSIG?qs=sGAEpiMZZMve4%2FbfQkoj%252BIdm5BjjR50fMw1zyWOlPKQ%3D"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>